<commit_message>
new path files in my directory exclude onedrive folder
</commit_message>
<xml_diff>
--- a/reports/Statistic_report_from_categorical_variables.xlsx
+++ b/reports/Statistic_report_from_categorical_variables.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,7 +511,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Partner</t>
+          <t>SeniorCitizen</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -526,16 +526,16 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>3641</v>
+        <v>5901</v>
       </c>
       <c r="F4" t="n">
-        <v>51.69672014766434</v>
+        <v>83.78531875621185</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Dependents</t>
+          <t>Partner</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -550,16 +550,16 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>4933</v>
+        <v>3641</v>
       </c>
       <c r="F5" t="n">
-        <v>70.04117563538264</v>
+        <v>51.69672014766434</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>PhoneService</t>
+          <t>Dependents</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -570,44 +570,44 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>6361</v>
+        <v>4933</v>
       </c>
       <c r="F6" t="n">
-        <v>90.31662643759762</v>
+        <v>70.04117563538264</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>MultipleLines</t>
+          <t>PhoneService</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>7043</v>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>3390</v>
+        <v>6361</v>
       </c>
       <c r="F7" t="n">
-        <v>48.13289791282124</v>
+        <v>90.31662643759762</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>InternetService</t>
+          <t>MultipleLines</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -618,20 +618,20 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Fiber optic</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>3096</v>
+        <v>3390</v>
       </c>
       <c r="F8" t="n">
-        <v>43.95854039471816</v>
+        <v>48.13289791282124</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>OnlineSecurity</t>
+          <t>InternetService</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -642,20 +642,20 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Fiber optic</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>3498</v>
+        <v>3096</v>
       </c>
       <c r="F9" t="n">
-        <v>49.66633536845094</v>
+        <v>43.95854039471816</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>OnlineBackup</t>
+          <t>OnlineSecurity</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -670,16 +670,16 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>3088</v>
+        <v>3498</v>
       </c>
       <c r="F10" t="n">
-        <v>43.84495243504188</v>
+        <v>49.66633536845094</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>DeviceProtection</t>
+          <t>OnlineBackup</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -694,16 +694,16 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>3095</v>
+        <v>3088</v>
       </c>
       <c r="F11" t="n">
-        <v>43.94434189975863</v>
+        <v>43.84495243504188</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>TechSupport</t>
+          <t>DeviceProtection</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -718,16 +718,16 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>3473</v>
+        <v>3095</v>
       </c>
       <c r="F12" t="n">
-        <v>49.31137299446259</v>
+        <v>43.94434189975863</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>StreamingTV</t>
+          <t>TechSupport</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -742,16 +742,16 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>2810</v>
+        <v>3473</v>
       </c>
       <c r="F13" t="n">
-        <v>39.89777083629135</v>
+        <v>49.31137299446259</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>StreamingMovies</t>
+          <t>StreamingTV</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -766,16 +766,16 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>2785</v>
+        <v>2810</v>
       </c>
       <c r="F14" t="n">
-        <v>39.542808462303</v>
+        <v>39.89777083629135</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Contract</t>
+          <t>StreamingMovies</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -786,85 +786,109 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Month-to-month</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>3875</v>
+        <v>2785</v>
       </c>
       <c r="F15" t="n">
-        <v>55.01916796819537</v>
+        <v>39.542808462303</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>PaperlessBilling</t>
+          <t>Contract</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>7043</v>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Month-to-month</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>4171</v>
+        <v>3875</v>
       </c>
       <c r="F16" t="n">
-        <v>59.22192247621753</v>
+        <v>55.01916796819537</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>PaymentMethod</t>
+          <t>PaperlessBilling</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>7043</v>
       </c>
       <c r="C17" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Electronic check</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>2365</v>
+        <v>4171</v>
       </c>
       <c r="F17" t="n">
-        <v>33.57944057929859</v>
+        <v>59.22192247621753</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
+          <t>PaymentMethod</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>7043</v>
+      </c>
+      <c r="C18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Electronic check</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>2365</v>
+      </c>
+      <c r="F18" t="n">
+        <v>33.57944057929859</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
           <t>Churn</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>7043</v>
-      </c>
-      <c r="C18" t="n">
+      <c r="B19" t="n">
+        <v>7043</v>
+      </c>
+      <c r="C19" t="n">
         <v>2</v>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
         <v>5174</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F19" t="n">
         <v>73.4630129206304</v>
       </c>
     </row>

</xml_diff>